<commit_message>
Destaque de cores planilha 2
</commit_message>
<xml_diff>
--- a/Simulador de investimentos imobiliários.xlsx
+++ b/Simulador de investimentos imobiliários.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aristóteles\Documents\Falta copiar - DIO Excel\Projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aristóteles\Documents\Projeto 1 - DIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7ACDB4-9272-40A4-B7AB-BD52DEB2CAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C01543-FFE6-4655-ABA4-97450CEDDFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="363" xr2:uid="{BC6D990E-6CAF-4AF5-B4DF-C82826CC5F3B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="363" activeTab="1" xr2:uid="{BC6D990E-6CAF-4AF5-B4DF-C82826CC5F3B}"/>
   </bookViews>
   <sheets>
     <sheet name="APP" sheetId="1" r:id="rId1"/>
@@ -217,14 +217,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -327,8 +319,16 @@
       <name val="Segoe UI Semibold"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -370,6 +370,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFDF79"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9797"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -613,170 +637,193 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="10" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="10" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="9" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="9" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="8" fontId="12" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="12" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="11" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="11" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="8" fontId="12" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="11" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="8" fontId="12" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="12" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="8" fontId="11" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="11" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="10" fontId="9" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="10" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -790,6 +837,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9797"/>
+      <color rgb="FFFFDF79"/>
       <color rgb="FF005CB8"/>
       <color rgb="FF0D530D"/>
       <color rgb="FF0A420A"/>
@@ -2359,7 +2408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243322A6-10E0-432E-9EA3-8CF0CA85E0A5}">
   <dimension ref="A5:F39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A33" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -2376,319 +2425,319 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:4" ht="85.5" customHeight="1" x14ac:dyDescent="1.65">
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
     </row>
     <row r="6" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.85">
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
     </row>
     <row r="7" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="45"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="39"/>
     </row>
     <row r="9" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="33">
+      <c r="C9" s="48"/>
+      <c r="D9" s="25">
         <v>5000</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="34">
+      <c r="C10" s="41"/>
+      <c r="D10" s="26">
         <v>0.01</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="8">
+      <c r="C11" s="50"/>
+      <c r="D11" s="7">
         <f>D9*30%</f>
         <v>1500</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="52"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="46"/>
     </row>
     <row r="14" spans="2:4" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="35">
+      <c r="C14" s="41"/>
+      <c r="D14" s="27">
         <v>500</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="36">
+      <c r="C15" s="41"/>
+      <c r="D15" s="28">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="47"/>
-      <c r="D16" s="37">
+      <c r="C16" s="41"/>
+      <c r="D16" s="29">
         <v>1.0789999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="6">
+      <c r="C17" s="43"/>
+      <c r="D17" s="5">
         <f>FV(taxa_mensal,qtd_anos*12,aporte*-1)</f>
         <v>41888.456999243819</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="7">
+      <c r="C18" s="33"/>
+      <c r="D18" s="6">
         <f>patrimonio*rendimento_carteira</f>
         <v>418.88456999243817</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>2</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="9">
         <f>FV($D$16,$A21*12,$D$14*-1)</f>
         <v>13613.813648822608</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="10">
         <f>C21*rendimento_carteira</f>
         <v>136.13813648822608</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>5</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="12">
         <f>FV($D$16,$A22*12,$D$14*-1)</f>
         <v>41888.456999243819</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="10">
         <f>C22*rendimento_carteira</f>
         <v>418.88456999243817</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>10</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="12">
         <f>FV($D$16,$A23*12,$D$14*-1)</f>
         <v>121642.1062650861</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="10">
         <f>C23*rendimento_carteira</f>
         <v>1216.4210626508609</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>20</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="12">
         <f>FV($D$16,$A24*12,$D$14*-1)</f>
         <v>562599.20004854025</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="10">
         <f>C24*rendimento_carteira</f>
         <v>5625.992000485403</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>30</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="14">
         <f>FV($D$16,$A25*12,$D$14*-1)</f>
         <v>2161084.8275023573</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="15">
         <f>C25*rendimento_carteira</f>
         <v>21610.848275023574</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="38" t="s">
+      <c r="C29" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="25"/>
+      <c r="D29" s="17"/>
     </row>
     <row r="30" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="39">
+      <c r="C30" s="31">
         <f>aporte</f>
         <v>500</v>
       </c>
-      <c r="D30" s="25"/>
+      <c r="D30" s="17"/>
     </row>
     <row r="31" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
     </row>
     <row r="32" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="27" t="s">
+      <c r="D32" s="19" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="29">
+      <c r="C33" s="21">
         <f>VLOOKUP($C$29&amp;"-"&amp;B33,Planilha2!$A$2:$D$20,4,FALSE)</f>
         <v>0.32</v>
       </c>
-      <c r="D33" s="30">
+      <c r="D33" s="22">
         <f>C33*$C$30</f>
         <v>160</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="29">
+      <c r="C34" s="21">
         <f>VLOOKUP($C$29&amp;"-"&amp;B34,Planilha2!$A$2:$D$20,4,FALSE)</f>
         <v>0.35</v>
       </c>
-      <c r="D34" s="30">
+      <c r="D34" s="22">
         <f t="shared" ref="D34:D38" si="0">C34*$C$30</f>
         <v>175</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="29">
+      <c r="C35" s="21">
         <f>VLOOKUP($C$29&amp;"-"&amp;B35,Planilha2!$A$2:$D$20,4,FALSE)</f>
         <v>0.08</v>
       </c>
-      <c r="D35" s="30">
+      <c r="D35" s="22">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="29">
+      <c r="C36" s="21">
         <f>VLOOKUP($C$29&amp;"-"&amp;B36,Planilha2!$A$2:$D$20,4,FALSE)</f>
         <v>0.05</v>
       </c>
-      <c r="D36" s="30">
+      <c r="D36" s="22">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="29">
+      <c r="C37" s="21">
         <f>VLOOKUP($C$29&amp;"-"&amp;B37,Planilha2!$A$2:$D$20,4,FALSE)</f>
         <v>0.1</v>
       </c>
-      <c r="D37" s="30">
+      <c r="D37" s="22">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="29">
+      <c r="C38" s="21">
         <f>VLOOKUP($C$29&amp;"-"&amp;B38,Planilha2!$A$2:$D$20,4,FALSE)</f>
         <v>0.1</v>
       </c>
-      <c r="D38" s="30">
+      <c r="D38" s="22">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="32">
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="24">
         <f>SUM(D33:D38)</f>
         <v>500</v>
       </c>
@@ -2722,8 +2771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{028B9867-F283-4300-8B92-8BF96E93660E}">
   <dimension ref="A2:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2732,287 +2781,287 @@
     <col min="2" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="51" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="53" t="str">
         <f>B3&amp;"-"&amp;C3</f>
         <v>Conservador-PAPEL</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="55">
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="53" t="str">
         <f t="shared" ref="A4:A8" si="0">B4&amp;"-"&amp;C4</f>
         <v>Conservador-TIJOLO</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="56">
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="53" t="str">
         <f t="shared" si="0"/>
         <v>Conservador-HIBRÍDOS</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="56">
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="53" t="str">
         <f t="shared" si="0"/>
         <v>Conservador-FOFs</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="56">
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="53" t="str">
         <f t="shared" si="0"/>
         <v>Conservador-DESENVOLVIMENTO</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="56">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="str">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="57" t="str">
         <f t="shared" si="0"/>
         <v>Conservador-HOTELARIAS</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="59">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="str">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="60" t="str">
         <f>B9&amp;"-"&amp;C9</f>
         <v>Moderado-PAPEL</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="62">
         <v>0.32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="str">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="60" t="str">
         <f t="shared" ref="A10:A13" si="1">B10&amp;"-"&amp;C10</f>
         <v>Moderado-TIJOLO</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="62">
         <v>0.35</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="str">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="60" t="str">
         <f t="shared" si="1"/>
         <v>Moderado-HIBRÍDOS</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="62">
         <v>0.08</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="str">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="60" t="str">
         <f t="shared" si="1"/>
         <v>Moderado-FOFs</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="62">
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="str">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="60" t="str">
         <f t="shared" si="1"/>
         <v>Moderado-DESENVOLVIMENTO</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="62">
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="str">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="63" t="str">
         <f>B14&amp;"-"&amp;C14</f>
         <v>Moderado-HOTELARIAS</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="65">
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="str">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="66" t="str">
         <f>B15&amp;"-"&amp;C15</f>
         <v>Agressivo-PAPEL</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="68">
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="str">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="66" t="str">
         <f t="shared" ref="A16:A20" si="2">B16&amp;"-"&amp;C16</f>
         <v>Agressivo-TIJOLO</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="68">
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="str">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="66" t="str">
         <f t="shared" si="2"/>
         <v>Agressivo-HIBRÍDOS</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="68">
         <v>0.05</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="str">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="66" t="str">
         <f t="shared" si="2"/>
         <v>Agressivo-FOFs</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="68">
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="str">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="66" t="str">
         <f t="shared" si="2"/>
         <v>Agressivo-DESENVOLVIMENTO</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="69">
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="str">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="66" t="str">
         <f t="shared" si="2"/>
         <v>Agressivo-HOTELARIAS</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="68">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>